<commit_message>
Add tests for empty cell for list type columns (and fix for .xlsx)
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/list_type.xlsx
+++ b/tests/testthat/sheets/list_type.xlsx
@@ -361,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -379,13 +379,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>42736</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix for multi-character strings
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/list_type.xlsx
+++ b/tests/testthat/sheets/list_type.xlsx
@@ -1,27 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greg/Desktop/readxl/tests/testthat/sheets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7485"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="18200" windowHeight="7480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>var1</t>
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -117,12 +133,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -152,12 +168,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -361,32 +377,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>42736</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -400,7 +421,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -412,7 +433,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add a logical cell to test sheet for list col type
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/list_type.xlsx
+++ b/tests/testthat/sheets/list_type.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greg/Desktop/readxl/tests/testthat/sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenny/rrr/readxl/tests/testthat/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="18200" windowHeight="7480"/>
+    <workbookView xWindow="15680" yWindow="1140" windowWidth="10000" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -377,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -408,6 +408,11 @@
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>